<commit_message>
DataFormatter to get the string value of each cell (Resolve the exception of INT cell value)
</commit_message>
<xml_diff>
--- a/src/main/java/ExcelUtils/ExcelConfigurationFile/confData.xlsx
+++ b/src/main/java/ExcelUtils/ExcelConfigurationFile/confData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
@@ -345,19 +351,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -365,12 +371,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>7896141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>